<commit_message>
MCD,MCD persistence, MLD, script BDD new version
</commit_message>
<xml_diff>
--- a/RepartitionTaches.xlsx
+++ b/RepartitionTaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Library/Mobile Documents/com~apple~CloudDocs/COURS_IG2I/COURS/LA2/POO/LeBonCoin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411B06A9-C614-874A-A4CE-117181344AFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F839B6-60B8-564B-B518-68575228BCEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20580" xr2:uid="{6B3C3676-455E-D242-9DDA-FB9D3C348B94}"/>
   </bookViews>
@@ -97,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +107,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,7 +450,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,16 +485,19 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
@@ -518,13 +528,14 @@
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">

</xml_diff>